<commit_message>
Made it clearer which plots used Collins approach versus budd in the Test1Aggregate file. Cleaned up a few of the graphs as well.
</commit_message>
<xml_diff>
--- a/Testing Data/Test1/Test1Aggregate.xlsx
+++ b/Testing Data/Test1/Test1Aggregate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Documents\EpiSci\SBL\SBL\Testing Data\Test1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16313910-14B4-4C3A-A968-9A5BEF2A12E1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D1F93DA-06B5-4789-AB3F-BA441AB9B257}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="3" xr2:uid="{2B4E69FC-4460-42BF-A1CF-3A680700B665}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{2B4E69FC-4460-42BF-A1CF-3A680700B665}"/>
   </bookViews>
   <sheets>
     <sheet name="Test1,Env2,Model0" sheetId="3" r:id="rId1"/>
@@ -238,8 +238,333 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Without budd (Collins)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model0'!$K$5:$K$32</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>4.3476459500745301E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.8224309129237288E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.0525654674514744E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.4083840341874199E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.0844984378707854E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1026229204862403E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.7822399474684594E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.7005306994137843E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.2451989389417104E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.026251808707749E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.9538672297878588E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model0'!$L$5:$L$32</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>1.4623531798272582E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.1564629477555135E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.3951751965601296E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.8675674118579546E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.506438154847578E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.9637881718409549E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.2341613891519478E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5139530113174056E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.9566048046029154E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.0971350938202025E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>6.9660151572416007E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model0'!$K$5:$K$32</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>4.3476459500745301E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.8224309129237288E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>4.0525654674514744E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>6.4083840341874199E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.0844984378707854E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>1.1026229204862403E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.7822399474684594E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.7005306994137843E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.2451989389417104E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>5.026251808707749E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.9538672297878588E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model0'!$L$5:$L$32</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>1.4623531798272582E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.1564629477555135E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>3.3951751965601296E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>5.8675674118579546E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>1.506438154847578E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>4.9637881718409549E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>5.2341613891519478E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.5139530113174056E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>4.9566048046029154E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.0971350938202025E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>6.9660151572416007E-3</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Test1,Env2,Model0'!$A$5:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Test1,Env2,Model0'!$H$5:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0.63059115111620356</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30545596188622615</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.30238993497521449</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.30503499832841718</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.30335315346767694</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30443051592189041</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30248178045339502</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.30578146512663384</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.30243105013808369</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.30509669664167655</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.30599656110273765</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-A741-439B-93D3-057E4C995539}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>With budd</c:v>
           </c:tx>
@@ -559,331 +884,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-A741-439B-93D3-057E4C995539}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Without budd</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="15875">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model0'!$K$5:$K$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>4.3476459500745301E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.8224309129237288E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.0525654674514744E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>6.4083840341874199E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.0844984378707854E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>1.1026229204862403E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>5.7822399474684594E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.7005306994137843E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>7.2451989389417104E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>5.026251808707749E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>7.9538672297878588E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model0'!$L$5:$L$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>1.4623531798272582E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.1564629477555135E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3.3951751965601296E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>5.8675674118579546E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.506438154847578E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4.9637881718409549E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>5.2341613891519478E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.5139530113174056E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>4.9566048046029154E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>3.0971350938202025E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>6.9660151572416007E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model0'!$K$5:$K$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>4.3476459500745301E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.8224309129237288E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>4.0525654674514744E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>6.4083840341874199E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.0844984378707854E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>1.1026229204862403E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>5.7822399474684594E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.7005306994137843E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>7.2451989389417104E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>5.026251808707749E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>7.9538672297878588E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model0'!$L$5:$L$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>1.4623531798272582E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.1564629477555135E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3.3951751965601296E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>5.8675674118579546E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>1.506438154847578E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4.9637881718409549E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>5.2341613891519478E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.5139530113174056E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>4.9566048046029154E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>3.0971350938202025E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>6.9660151572416007E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Test1,Env2,Model0'!$A$5:$A$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Test1,Env2,Model0'!$H$5:$H$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0.63059115111620356</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.30545596188622615</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.30238993497521449</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.30503499832841718</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.30335315346767694</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.30443051592189041</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.30248178045339502</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.30578146512663384</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.30243105013808369</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.30509669664167655</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.30599656110273765</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-A741-439B-93D3-057E4C995539}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1302,8 +1302,176 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Without budd (Collins)</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="stdErr"/>
+            <c:noEndCap val="0"/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Test1,Env2,Model1'!$A$5:$A$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>70263</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Test1,Env2,Model1'!$H$5:$H$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0.68986317635955463</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27084666907438654</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26790267387550237</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.25870510532814617</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26350376609820475</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26398741996863295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.26173639015486094</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25934600816257064</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2610294340416458</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.2647473798743184</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.26191090830068819</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.25996101006327216</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.25887656111404284</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.2599547973889107</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.26045862779384132</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.259558254634768</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-71DC-4927-98F6-C5C62343C06F}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
           <c:idx val="0"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>With budd</c:v>
           </c:tx>
@@ -1713,421 +1881,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-71DC-4927-98F6-C5C62343C06F}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Without budd</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="15875">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model1'!$K$5:$K$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>1.8506985403558773E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>6.2760449472337165E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5.9633324971137824E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.3334116405746888E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.5626665137306057E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>5.5933516362715041E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>9.0917732321813549E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>4.1369701975173534E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>1.2873343909408641E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>2.6173440825178473E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.3965887735091238E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>2.6461036630554546E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>4.8118615076789828E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>6.6226459877924415E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>8.0227674544250394E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>6.8203515827919836E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model1'!$L$5:$L$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>1.9475510856852285E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.2125386705833241E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9.9782169550388655E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.0360572160262954E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8.8494466447309184E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4.9106834208818007E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7.57277754678648E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>2.5765346198099448E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>5.270591226743504E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>4.1708462485460784E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>1.9892446932505692E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>5.8775924613925778E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>3.5940876614616868E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>4.5330956587508187E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>4.4823346520367346E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4.6095007811313149E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model1'!$K$5:$K$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>1.8506985403558773E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>6.2760449472337165E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>5.9633324971137824E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.3334116405746888E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3.5626665137306057E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>5.5933516362715041E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>9.0917732321813549E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>4.1369701975173534E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>1.2873343909408641E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>2.6173440825178473E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.3965887735091238E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>2.6461036630554546E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>4.8118615076789828E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>6.6226459877924415E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>8.0227674544250394E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>6.8203515827919836E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model1'!$L$5:$L$32</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>1.9475510856852285E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>1.2125386705833241E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>9.9782169550388655E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.0360572160262954E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>8.8494466447309184E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>4.9106834208818007E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7.57277754678648E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>2.5765346198099448E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>5.270591226743504E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>4.1708462485460784E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>1.9892446932505692E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>5.8775924613925778E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>3.5940876614616868E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>4.5330956587508187E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>4.4823346520367346E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>4.6095007811313149E-3</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Test1,Env2,Model1'!$A$5:$A$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>70263</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Test1,Env2,Model1'!$H$5:$H$32</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0.68986317635955463</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.27084666907438654</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.26790267387550237</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.25870510532814617</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.26350376609820475</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.26398741996863295</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>0.26173639015486094</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.25934600816257064</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.2610294340416458</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>0.2647473798743184</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.26191090830068819</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.25996101006327216</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.25887656111404284</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>0.2599547973889107</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>0.26045862779384132</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>0.259558254634768</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-71DC-4927-98F6-C5C62343C06F}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2546,641 +2299,10 @@
         <c:scatterStyle val="lineMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>With budd</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:noFill/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:errBars>
-            <c:errDir val="x"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model2'!$I$41:$I$68</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>0.65564727813074009</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.17121379190447522</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.14947191945281835</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>0.12669043805260077</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>0.12143039140483111</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>0.12590756195532368</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>0.13094038112484133</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>0.12314099146818808</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>0.11616672660385111</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>0.11964968111296817</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>0.11813228196117424</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>0.1153553204061179</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>0.11904813811538423</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>0.11779058480724172</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>0.12175346783933219</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>0.11486732760285613</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>0.12027878537929701</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>0.11858769496918496</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>0.11586210826727643</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>0.11770675149515496</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>0.11543658368835599</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>0.11814605262891359</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>0.11625006496560364</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>0.11220927365710698</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>0.11005032730412845</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>0.1120385076795475</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>0.11295109543613066</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>0.11179484354681317</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model2'!$J$41:$J$68</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>0.64177566299251054</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>0.15741455225269102</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>0.10264617716353634</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>7.9713555336000372E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6.8417949086619065E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>6.794474290673061E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>7.0917822402890768E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>7.8556081221673665E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>7.9971420723080847E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>8.0014954545267705E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>7.4359327357199523E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>7.4082667872737526E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>7.1604680828084563E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>7.0431076365544146E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>7.0151991068238412E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>6.7781123651443023E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>6.6308122882500528E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>6.6511157585873573E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>6.7591309555555715E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>6.6131741889763632E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>6.4811161956278465E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>6.5407744466320375E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>6.5771184167855712E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>6.374845427512478E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>6.3561673686044123E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>6.4030640969432437E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>7.1592194942437237E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>7.0410884873810017E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:errBars>
-            <c:errDir val="y"/>
-            <c:errBarType val="both"/>
-            <c:errValType val="cust"/>
-            <c:noEndCap val="0"/>
-            <c:plus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model2'!$K$41:$K$68</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>9.9662169462533257E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>5.5491574893199447E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.0936530715775559E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1.8319031368362451E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.3668637579569884E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>3.3058271892130953E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>4.0169181120591091E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>3.139803953842743E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>2.7206390613107589E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>3.0845400715746887E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>3.3594694922534141E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>3.0076001906819055E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>3.5369052860922415E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>3.4448446969887803E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>3.9143908165162444E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>3.3825076382788338E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>3.8633964396450005E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>3.71198650823205E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>3.6374808161220351E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>3.8129539287619266E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>3.7104091170561015E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>3.829802220703693E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>3.6956190222497395E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>3.4896852900258624E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>3.2319285505345324E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>3.2375531935478277E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>2.9513680815133003E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>2.8641917534063158E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:plus>
-            <c:minus>
-              <c:numRef>
-                <c:f>'Test1,Env2,Model2'!$L$41:$L$68</c:f>
-                <c:numCache>
-                  <c:formatCode>General</c:formatCode>
-                  <c:ptCount val="28"/>
-                  <c:pt idx="0">
-                    <c:v>3.9053981919762171E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>8.2500821624642562E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2.5889211573506446E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2.865785134823795E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2.9343804738642162E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>2.490454715646212E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>1.9853377601359468E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>1.3186870708086981E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>8.9889152676626699E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>8.7893258519535777E-3</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>1.017825968144058E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>1.1196650626561319E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>1.207440442637725E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="13">
-                    <c:v>1.2911061471809773E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="14">
-                    <c:v>1.2457568605931335E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="15">
-                    <c:v>1.326112756862477E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="16">
-                    <c:v>1.5336698100346477E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="17">
-                    <c:v>1.4956672300990889E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="18">
-                    <c:v>1.1895990550500363E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="19">
-                    <c:v>1.344547031777206E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="20">
-                    <c:v>1.3521330561516512E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="21">
-                    <c:v>1.4440285955556284E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="22">
-                    <c:v>1.3522690575250532E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="23">
-                    <c:v>1.3563966481723574E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="24">
-                    <c:v>1.4169368112739E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="25">
-                    <c:v>1.5632334774636783E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="26">
-                    <c:v>1.184521967856042E-2</c:v>
-                  </c:pt>
-                  <c:pt idx="27">
-                    <c:v>1.2742041138939994E-2</c:v>
-                  </c:pt>
-                </c:numCache>
-              </c:numRef>
-            </c:minus>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:round/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:errBars>
-          <c:xVal>
-            <c:numRef>
-              <c:f>'Test1,Env2,Model2'!$A$41:$A$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10000</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>15000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>20000</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>25000</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>30000</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>35000</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40000</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>45000</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>50000</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>55000</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>60000</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>65000</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>70000</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>75000</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>80000</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>85000</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>90000</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>95000</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>100000</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>105000</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>110000</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>115000</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>120000</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>125000</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>130000</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>131189</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>'Test1,Env2,Model2'!$H$41:$H$68</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="28"/>
-                <c:pt idx="0">
-                  <c:v>0.64568106118448676</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.16566463441515528</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.12853538873704279</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.10837140668423832</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>9.7761753825261227E-2</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.284929006319273E-2</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>9.0771200004250235E-2</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>9.1742951929760647E-2</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>8.8960335990743516E-2</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>8.8804280397221283E-2</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>8.4537587038640102E-2</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>8.5279318499298845E-2</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.3679085254461813E-2</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>8.3342137837353919E-2</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>8.2609559674169747E-2</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>8.1042251220067793E-2</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>8.1644820982847005E-2</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>8.1467829886864462E-2</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>7.9487300106056077E-2</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>7.9577212207535691E-2</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>7.8332492517794977E-2</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.9848030421876659E-2</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>7.9293874743106244E-2</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>7.7312420756848355E-2</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>7.7731041798783124E-2</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>7.966297574406922E-2</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>8.3437414620997657E-2</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>8.3152926012750011E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:yVal>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-B838-4CEA-AEA0-3DAE6F9BA211}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Without budd</c:v>
+            <c:v>Without budd (Collins)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -3828,6 +2950,637 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B838-4CEA-AEA0-3DAE6F9BA211}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>With budd</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model2'!$I$41:$I$68</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>0.65564727813074009</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.17121379190447522</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.14947191945281835</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.12669043805260077</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.12143039140483111</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.12590756195532368</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.13094038112484133</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.12314099146818808</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.11616672660385111</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>0.11964968111296817</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>0.11813228196117424</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>0.1153553204061179</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>0.11904813811538423</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>0.11779058480724172</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>0.12175346783933219</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>0.11486732760285613</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>0.12027878537929701</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>0.11858769496918496</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>0.11586210826727643</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>0.11770675149515496</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>0.11543658368835599</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>0.11814605262891359</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>0.11625006496560364</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>0.11220927365710698</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>0.11005032730412845</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>0.1120385076795475</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>0.11295109543613066</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>0.11179484354681317</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model2'!$J$41:$J$68</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>0.64177566299251054</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.15741455225269102</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.10264617716353634</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>7.9713555336000372E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>6.8417949086619065E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6.794474290673061E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>7.0917822402890768E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>7.8556081221673665E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>7.9971420723080847E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.0014954545267705E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>7.4359327357199523E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>7.4082667872737526E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>7.1604680828084563E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>7.0431076365544146E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>7.0151991068238412E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>6.7781123651443023E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>6.6308122882500528E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>6.6511157585873573E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>6.7591309555555715E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>6.6131741889763632E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>6.4811161956278465E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>6.5407744466320375E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>6.5771184167855712E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>6.374845427512478E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>6.3561673686044123E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>6.4030640969432437E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>7.1592194942437237E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>7.0410884873810017E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model2'!$K$41:$K$68</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>9.9662169462533257E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>5.5491574893199447E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.0936530715775559E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1.8319031368362451E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.3668637579569884E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3.3058271892130953E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>4.0169181120591091E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>3.139803953842743E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>2.7206390613107589E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>3.0845400715746887E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>3.3594694922534141E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>3.0076001906819055E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>3.5369052860922415E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>3.4448446969887803E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>3.9143908165162444E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>3.3825076382788338E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>3.8633964396450005E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>3.71198650823205E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>3.6374808161220351E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>3.8129539287619266E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>3.7104091170561015E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>3.829802220703693E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>3.6956190222497395E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>3.4896852900258624E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>3.2319285505345324E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>3.2375531935478277E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>2.9513680815133003E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>2.8641917534063158E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Test1,Env2,Model2'!$L$41:$L$68</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="28"/>
+                  <c:pt idx="0">
+                    <c:v>3.9053981919762171E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>8.2500821624642562E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>2.5889211573506446E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>2.865785134823795E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>2.9343804738642162E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2.490454715646212E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1.9853377601359468E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1.3186870708086981E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>8.9889152676626699E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>8.7893258519535777E-3</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>1.017825968144058E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>1.1196650626561319E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>1.207440442637725E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>1.2911061471809773E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>1.2457568605931335E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>1.326112756862477E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>1.5336698100346477E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>1.4956672300990889E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>1.1895990550500363E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>1.344547031777206E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="20">
+                    <c:v>1.3521330561516512E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="21">
+                    <c:v>1.4440285955556284E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="22">
+                    <c:v>1.3522690575250532E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="23">
+                    <c:v>1.3563966481723574E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="24">
+                    <c:v>1.4169368112739E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="25">
+                    <c:v>1.5632334774636783E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="26">
+                    <c:v>1.184521967856042E-2</c:v>
+                  </c:pt>
+                  <c:pt idx="27">
+                    <c:v>1.2742041138939994E-2</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Test1,Env2,Model2'!$A$41:$A$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15000</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>25000</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>30000</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>40000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45000</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>50000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>55000</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>60000</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>65000</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>70000</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>75000</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>80000</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>85000</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>90000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>95000</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>105000</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>110000</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>115000</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>120000</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>125000</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>130000</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>131189</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Test1,Env2,Model2'!$H$41:$H$68</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="28"/>
+                <c:pt idx="0">
+                  <c:v>0.64568106118448676</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.16566463441515528</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.12853538873704279</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.10837140668423832</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>9.7761753825261227E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>9.284929006319273E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>9.0771200004250235E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.1742951929760647E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.8960335990743516E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>8.8804280397221283E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.4537587038640102E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>8.5279318499298845E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>8.3679085254461813E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.3342137837353919E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>8.2609559674169747E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>8.1042251220067793E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.1644820982847005E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.1467829886864462E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7.9487300106056077E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>7.9577212207535691E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>7.8332492517794977E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>7.9848030421876659E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>7.9293874743106244E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>7.7312420756848355E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>7.7731041798783124E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>7.966297574406922E-2</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>8.3437414620997657E-2</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>8.3152926012750011E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B838-4CEA-AEA0-3DAE6F9BA211}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4249,7 +4002,7 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Without budd</c:v>
+            <c:v>Without budd (Collins)</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -7765,15 +7518,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>200025</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8186,8 +7939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CDB7529A-9826-44A5-B186-D7D0D5B50388}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37:L51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9469,8 +9222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{401FBB92-91A7-46B8-AB24-03D49E3AD615}">
   <dimension ref="A1:L68"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:L56"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="V28" sqref="V28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12343,23 +12096,23 @@
         <v>0.64359122963641424</v>
       </c>
       <c r="H41">
-        <f>AVERAGE(B41:F41)</f>
+        <f t="shared" ref="H41:H68" si="5">AVERAGE(B41:F41)</f>
         <v>0.64568106118448676</v>
       </c>
       <c r="I41">
-        <f>MAX(B41:F41)</f>
+        <f t="shared" ref="I41:I68" si="6">MAX(B41:F41)</f>
         <v>0.65564727813074009</v>
       </c>
       <c r="J41">
-        <f>MIN(B41:F41)</f>
+        <f t="shared" ref="J41:J68" si="7">MIN(B41:F41)</f>
         <v>0.64177566299251054</v>
       </c>
       <c r="K41">
-        <f>ABS(I41-H41)</f>
+        <f t="shared" ref="K41:K68" si="8">ABS(I41-H41)</f>
         <v>9.9662169462533257E-3</v>
       </c>
       <c r="L41">
-        <f>ABS(H41-J41)</f>
+        <f t="shared" ref="L41:L68" si="9">ABS(H41-J41)</f>
         <v>3.9053981919762171E-3</v>
       </c>
     </row>
@@ -12383,23 +12136,23 @@
         <v>0.16992503113262636</v>
       </c>
       <c r="H42">
-        <f>AVERAGE(B42:F42)</f>
+        <f t="shared" si="5"/>
         <v>0.16566463441515528</v>
       </c>
       <c r="I42">
-        <f>MAX(B42:F42)</f>
+        <f t="shared" si="6"/>
         <v>0.17121379190447522</v>
       </c>
       <c r="J42">
-        <f>MIN(B42:F42)</f>
+        <f t="shared" si="7"/>
         <v>0.15741455225269102</v>
       </c>
       <c r="K42">
-        <f>ABS(I42-H42)</f>
+        <f t="shared" si="8"/>
         <v>5.5491574893199447E-3</v>
       </c>
       <c r="L42">
-        <f>ABS(H42-J42)</f>
+        <f t="shared" si="9"/>
         <v>8.2500821624642562E-3</v>
       </c>
     </row>
@@ -12423,23 +12176,23 @@
         <v>0.14947191945281835</v>
       </c>
       <c r="H43">
-        <f>AVERAGE(B43:F43)</f>
+        <f t="shared" si="5"/>
         <v>0.12853538873704279</v>
       </c>
       <c r="I43">
-        <f>MAX(B43:F43)</f>
+        <f t="shared" si="6"/>
         <v>0.14947191945281835</v>
       </c>
       <c r="J43">
-        <f>MIN(B43:F43)</f>
+        <f t="shared" si="7"/>
         <v>0.10264617716353634</v>
       </c>
       <c r="K43">
-        <f>ABS(I43-H43)</f>
+        <f t="shared" si="8"/>
         <v>2.0936530715775559E-2</v>
       </c>
       <c r="L43">
-        <f>ABS(H43-J43)</f>
+        <f t="shared" si="9"/>
         <v>2.5889211573506446E-2</v>
       </c>
     </row>
@@ -12463,23 +12216,23 @@
         <v>0.12669043805260077</v>
       </c>
       <c r="H44">
-        <f>AVERAGE(B44:F44)</f>
+        <f t="shared" si="5"/>
         <v>0.10837140668423832</v>
       </c>
       <c r="I44">
-        <f>MAX(B44:F44)</f>
+        <f t="shared" si="6"/>
         <v>0.12669043805260077</v>
       </c>
       <c r="J44">
-        <f>MIN(B44:F44)</f>
+        <f t="shared" si="7"/>
         <v>7.9713555336000372E-2</v>
       </c>
       <c r="K44">
-        <f>ABS(I44-H44)</f>
+        <f t="shared" si="8"/>
         <v>1.8319031368362451E-2</v>
       </c>
       <c r="L44">
-        <f>ABS(H44-J44)</f>
+        <f t="shared" si="9"/>
         <v>2.865785134823795E-2</v>
       </c>
     </row>
@@ -12503,23 +12256,23 @@
         <v>0.12143039140483111</v>
       </c>
       <c r="H45">
-        <f>AVERAGE(B45:F45)</f>
+        <f t="shared" si="5"/>
         <v>9.7761753825261227E-2</v>
       </c>
       <c r="I45">
-        <f>MAX(B45:F45)</f>
+        <f t="shared" si="6"/>
         <v>0.12143039140483111</v>
       </c>
       <c r="J45">
-        <f>MIN(B45:F45)</f>
+        <f t="shared" si="7"/>
         <v>6.8417949086619065E-2</v>
       </c>
       <c r="K45">
-        <f>ABS(I45-H45)</f>
+        <f t="shared" si="8"/>
         <v>2.3668637579569884E-2</v>
       </c>
       <c r="L45">
-        <f>ABS(H45-J45)</f>
+        <f t="shared" si="9"/>
         <v>2.9343804738642162E-2</v>
       </c>
     </row>
@@ -12543,23 +12296,23 @@
         <v>0.12590756195532368</v>
       </c>
       <c r="H46">
-        <f>AVERAGE(B46:F46)</f>
+        <f t="shared" si="5"/>
         <v>9.284929006319273E-2</v>
       </c>
       <c r="I46">
-        <f>MAX(B46:F46)</f>
+        <f t="shared" si="6"/>
         <v>0.12590756195532368</v>
       </c>
       <c r="J46">
-        <f>MIN(B46:F46)</f>
+        <f t="shared" si="7"/>
         <v>6.794474290673061E-2</v>
       </c>
       <c r="K46">
-        <f>ABS(I46-H46)</f>
+        <f t="shared" si="8"/>
         <v>3.3058271892130953E-2</v>
       </c>
       <c r="L46">
-        <f>ABS(H46-J46)</f>
+        <f t="shared" si="9"/>
         <v>2.490454715646212E-2</v>
       </c>
     </row>
@@ -12583,23 +12336,23 @@
         <v>0.13094038112484133</v>
       </c>
       <c r="H47">
-        <f>AVERAGE(B47:F47)</f>
+        <f t="shared" si="5"/>
         <v>9.0771200004250235E-2</v>
       </c>
       <c r="I47">
-        <f>MAX(B47:F47)</f>
+        <f t="shared" si="6"/>
         <v>0.13094038112484133</v>
       </c>
       <c r="J47">
-        <f>MIN(B47:F47)</f>
+        <f t="shared" si="7"/>
         <v>7.0917822402890768E-2</v>
       </c>
       <c r="K47">
-        <f>ABS(I47-H47)</f>
+        <f t="shared" si="8"/>
         <v>4.0169181120591091E-2</v>
       </c>
       <c r="L47">
-        <f>ABS(H47-J47)</f>
+        <f t="shared" si="9"/>
         <v>1.9853377601359468E-2</v>
       </c>
     </row>
@@ -12623,23 +12376,23 @@
         <v>0.12314099146818808</v>
       </c>
       <c r="H48">
-        <f>AVERAGE(B48:F48)</f>
+        <f t="shared" si="5"/>
         <v>9.1742951929760647E-2</v>
       </c>
       <c r="I48">
-        <f>MAX(B48:F48)</f>
+        <f t="shared" si="6"/>
         <v>0.12314099146818808</v>
       </c>
       <c r="J48">
-        <f>MIN(B48:F48)</f>
+        <f t="shared" si="7"/>
         <v>7.8556081221673665E-2</v>
       </c>
       <c r="K48">
-        <f>ABS(I48-H48)</f>
+        <f t="shared" si="8"/>
         <v>3.139803953842743E-2</v>
       </c>
       <c r="L48">
-        <f>ABS(H48-J48)</f>
+        <f t="shared" si="9"/>
         <v>1.3186870708086981E-2</v>
       </c>
     </row>
@@ -12663,23 +12416,23 @@
         <v>0.11616672660385111</v>
       </c>
       <c r="H49">
-        <f>AVERAGE(B49:F49)</f>
+        <f t="shared" si="5"/>
         <v>8.8960335990743516E-2</v>
       </c>
       <c r="I49">
-        <f>MAX(B49:F49)</f>
+        <f t="shared" si="6"/>
         <v>0.11616672660385111</v>
       </c>
       <c r="J49">
-        <f>MIN(B49:F49)</f>
+        <f t="shared" si="7"/>
         <v>7.9971420723080847E-2</v>
       </c>
       <c r="K49">
-        <f>ABS(I49-H49)</f>
+        <f t="shared" si="8"/>
         <v>2.7206390613107589E-2</v>
       </c>
       <c r="L49">
-        <f>ABS(H49-J49)</f>
+        <f t="shared" si="9"/>
         <v>8.9889152676626699E-3</v>
       </c>
     </row>
@@ -12703,23 +12456,23 @@
         <v>0.11964968111296817</v>
       </c>
       <c r="H50">
-        <f>AVERAGE(B50:F50)</f>
+        <f t="shared" si="5"/>
         <v>8.8804280397221283E-2</v>
       </c>
       <c r="I50">
-        <f>MAX(B50:F50)</f>
+        <f t="shared" si="6"/>
         <v>0.11964968111296817</v>
       </c>
       <c r="J50">
-        <f>MIN(B50:F50)</f>
+        <f t="shared" si="7"/>
         <v>8.0014954545267705E-2</v>
       </c>
       <c r="K50">
-        <f>ABS(I50-H50)</f>
+        <f t="shared" si="8"/>
         <v>3.0845400715746887E-2</v>
       </c>
       <c r="L50">
-        <f>ABS(H50-J50)</f>
+        <f t="shared" si="9"/>
         <v>8.7893258519535777E-3</v>
       </c>
     </row>
@@ -12743,23 +12496,23 @@
         <v>0.11813228196117424</v>
       </c>
       <c r="H51">
-        <f>AVERAGE(B51:F51)</f>
+        <f t="shared" si="5"/>
         <v>8.4537587038640102E-2</v>
       </c>
       <c r="I51">
-        <f>MAX(B51:F51)</f>
+        <f t="shared" si="6"/>
         <v>0.11813228196117424</v>
       </c>
       <c r="J51">
-        <f>MIN(B51:F51)</f>
+        <f t="shared" si="7"/>
         <v>7.4359327357199523E-2</v>
       </c>
       <c r="K51">
-        <f>ABS(I51-H51)</f>
+        <f t="shared" si="8"/>
         <v>3.3594694922534141E-2</v>
       </c>
       <c r="L51">
-        <f>ABS(H51-J51)</f>
+        <f t="shared" si="9"/>
         <v>1.017825968144058E-2</v>
       </c>
     </row>
@@ -12783,23 +12536,23 @@
         <v>0.1153553204061179</v>
       </c>
       <c r="H52">
-        <f>AVERAGE(B52:F52)</f>
+        <f t="shared" si="5"/>
         <v>8.5279318499298845E-2</v>
       </c>
       <c r="I52">
-        <f>MAX(B52:F52)</f>
+        <f t="shared" si="6"/>
         <v>0.1153553204061179</v>
       </c>
       <c r="J52">
-        <f>MIN(B52:F52)</f>
+        <f t="shared" si="7"/>
         <v>7.4082667872737526E-2</v>
       </c>
       <c r="K52">
-        <f>ABS(I52-H52)</f>
+        <f t="shared" si="8"/>
         <v>3.0076001906819055E-2</v>
       </c>
       <c r="L52">
-        <f>ABS(H52-J52)</f>
+        <f t="shared" si="9"/>
         <v>1.1196650626561319E-2</v>
       </c>
     </row>
@@ -12823,23 +12576,23 @@
         <v>0.11904813811538423</v>
       </c>
       <c r="H53">
-        <f>AVERAGE(B53:F53)</f>
+        <f t="shared" si="5"/>
         <v>8.3679085254461813E-2</v>
       </c>
       <c r="I53">
-        <f>MAX(B53:F53)</f>
+        <f t="shared" si="6"/>
         <v>0.11904813811538423</v>
       </c>
       <c r="J53">
-        <f>MIN(B53:F53)</f>
+        <f t="shared" si="7"/>
         <v>7.1604680828084563E-2</v>
       </c>
       <c r="K53">
-        <f>ABS(I53-H53)</f>
+        <f t="shared" si="8"/>
         <v>3.5369052860922415E-2</v>
       </c>
       <c r="L53">
-        <f>ABS(H53-J53)</f>
+        <f t="shared" si="9"/>
         <v>1.207440442637725E-2</v>
       </c>
     </row>
@@ -12863,23 +12616,23 @@
         <v>0.11779058480724172</v>
       </c>
       <c r="H54">
-        <f>AVERAGE(B54:F54)</f>
+        <f t="shared" si="5"/>
         <v>8.3342137837353919E-2</v>
       </c>
       <c r="I54">
-        <f>MAX(B54:F54)</f>
+        <f t="shared" si="6"/>
         <v>0.11779058480724172</v>
       </c>
       <c r="J54">
-        <f>MIN(B54:F54)</f>
+        <f t="shared" si="7"/>
         <v>7.0431076365544146E-2</v>
       </c>
       <c r="K54">
-        <f>ABS(I54-H54)</f>
+        <f t="shared" si="8"/>
         <v>3.4448446969887803E-2</v>
       </c>
       <c r="L54">
-        <f>ABS(H54-J54)</f>
+        <f t="shared" si="9"/>
         <v>1.2911061471809773E-2</v>
       </c>
     </row>
@@ -12903,23 +12656,23 @@
         <v>0.12175346783933219</v>
       </c>
       <c r="H55">
-        <f>AVERAGE(B55:F55)</f>
+        <f t="shared" si="5"/>
         <v>8.2609559674169747E-2</v>
       </c>
       <c r="I55">
-        <f>MAX(B55:F55)</f>
+        <f t="shared" si="6"/>
         <v>0.12175346783933219</v>
       </c>
       <c r="J55">
-        <f>MIN(B55:F55)</f>
+        <f t="shared" si="7"/>
         <v>7.0151991068238412E-2</v>
       </c>
       <c r="K55">
-        <f>ABS(I55-H55)</f>
+        <f t="shared" si="8"/>
         <v>3.9143908165162444E-2</v>
       </c>
       <c r="L55">
-        <f>ABS(H55-J55)</f>
+        <f t="shared" si="9"/>
         <v>1.2457568605931335E-2</v>
       </c>
     </row>
@@ -12943,23 +12696,23 @@
         <v>0.11486732760285613</v>
       </c>
       <c r="H56">
-        <f>AVERAGE(B56:F56)</f>
+        <f t="shared" si="5"/>
         <v>8.1042251220067793E-2</v>
       </c>
       <c r="I56">
-        <f>MAX(B56:F56)</f>
+        <f t="shared" si="6"/>
         <v>0.11486732760285613</v>
       </c>
       <c r="J56">
-        <f>MIN(B56:F56)</f>
+        <f t="shared" si="7"/>
         <v>6.7781123651443023E-2</v>
       </c>
       <c r="K56">
-        <f>ABS(I56-H56)</f>
+        <f t="shared" si="8"/>
         <v>3.3825076382788338E-2</v>
       </c>
       <c r="L56">
-        <f>ABS(H56-J56)</f>
+        <f t="shared" si="9"/>
         <v>1.326112756862477E-2</v>
       </c>
     </row>
@@ -12983,23 +12736,23 @@
         <v>0.12027878537929701</v>
       </c>
       <c r="H57">
-        <f>AVERAGE(B57:F57)</f>
+        <f t="shared" si="5"/>
         <v>8.1644820982847005E-2</v>
       </c>
       <c r="I57">
-        <f>MAX(B57:F57)</f>
+        <f t="shared" si="6"/>
         <v>0.12027878537929701</v>
       </c>
       <c r="J57">
-        <f>MIN(B57:F57)</f>
+        <f t="shared" si="7"/>
         <v>6.6308122882500528E-2</v>
       </c>
       <c r="K57">
-        <f>ABS(I57-H57)</f>
+        <f t="shared" si="8"/>
         <v>3.8633964396450005E-2</v>
       </c>
       <c r="L57">
-        <f>ABS(H57-J57)</f>
+        <f t="shared" si="9"/>
         <v>1.5336698100346477E-2</v>
       </c>
     </row>
@@ -13023,23 +12776,23 @@
         <v>0.11858769496918496</v>
       </c>
       <c r="H58">
-        <f>AVERAGE(B58:F58)</f>
+        <f t="shared" si="5"/>
         <v>8.1467829886864462E-2</v>
       </c>
       <c r="I58">
-        <f>MAX(B58:F58)</f>
+        <f t="shared" si="6"/>
         <v>0.11858769496918496</v>
       </c>
       <c r="J58">
-        <f>MIN(B58:F58)</f>
+        <f t="shared" si="7"/>
         <v>6.6511157585873573E-2</v>
       </c>
       <c r="K58">
-        <f>ABS(I58-H58)</f>
+        <f t="shared" si="8"/>
         <v>3.71198650823205E-2</v>
       </c>
       <c r="L58">
-        <f>ABS(H58-J58)</f>
+        <f t="shared" si="9"/>
         <v>1.4956672300990889E-2</v>
       </c>
     </row>
@@ -13063,23 +12816,23 @@
         <v>0.11586210826727643</v>
       </c>
       <c r="H59">
-        <f>AVERAGE(B59:F59)</f>
+        <f t="shared" si="5"/>
         <v>7.9487300106056077E-2</v>
       </c>
       <c r="I59">
-        <f>MAX(B59:F59)</f>
+        <f t="shared" si="6"/>
         <v>0.11586210826727643</v>
       </c>
       <c r="J59">
-        <f>MIN(B59:F59)</f>
+        <f t="shared" si="7"/>
         <v>6.7591309555555715E-2</v>
       </c>
       <c r="K59">
-        <f>ABS(I59-H59)</f>
+        <f t="shared" si="8"/>
         <v>3.6374808161220351E-2</v>
       </c>
       <c r="L59">
-        <f>ABS(H59-J59)</f>
+        <f t="shared" si="9"/>
         <v>1.1895990550500363E-2</v>
       </c>
     </row>
@@ -13103,23 +12856,23 @@
         <v>0.11770675149515496</v>
       </c>
       <c r="H60">
-        <f>AVERAGE(B60:F60)</f>
+        <f t="shared" si="5"/>
         <v>7.9577212207535691E-2</v>
       </c>
       <c r="I60">
-        <f>MAX(B60:F60)</f>
+        <f t="shared" si="6"/>
         <v>0.11770675149515496</v>
       </c>
       <c r="J60">
-        <f>MIN(B60:F60)</f>
+        <f t="shared" si="7"/>
         <v>6.6131741889763632E-2</v>
       </c>
       <c r="K60">
-        <f>ABS(I60-H60)</f>
+        <f t="shared" si="8"/>
         <v>3.8129539287619266E-2</v>
       </c>
       <c r="L60">
-        <f>ABS(H60-J60)</f>
+        <f t="shared" si="9"/>
         <v>1.344547031777206E-2</v>
       </c>
     </row>
@@ -13143,23 +12896,23 @@
         <v>0.11543658368835599</v>
       </c>
       <c r="H61">
-        <f>AVERAGE(B61:F61)</f>
+        <f t="shared" si="5"/>
         <v>7.8332492517794977E-2</v>
       </c>
       <c r="I61">
-        <f>MAX(B61:F61)</f>
+        <f t="shared" si="6"/>
         <v>0.11543658368835599</v>
       </c>
       <c r="J61">
-        <f>MIN(B61:F61)</f>
+        <f t="shared" si="7"/>
         <v>6.4811161956278465E-2</v>
       </c>
       <c r="K61">
-        <f>ABS(I61-H61)</f>
+        <f t="shared" si="8"/>
         <v>3.7104091170561015E-2</v>
       </c>
       <c r="L61">
-        <f>ABS(H61-J61)</f>
+        <f t="shared" si="9"/>
         <v>1.3521330561516512E-2</v>
       </c>
     </row>
@@ -13183,23 +12936,23 @@
         <v>0.11814605262891359</v>
       </c>
       <c r="H62">
-        <f>AVERAGE(B62:F62)</f>
+        <f t="shared" si="5"/>
         <v>7.9848030421876659E-2</v>
       </c>
       <c r="I62">
-        <f>MAX(B62:F62)</f>
+        <f t="shared" si="6"/>
         <v>0.11814605262891359</v>
       </c>
       <c r="J62">
-        <f>MIN(B62:F62)</f>
+        <f t="shared" si="7"/>
         <v>6.5407744466320375E-2</v>
       </c>
       <c r="K62">
-        <f>ABS(I62-H62)</f>
+        <f t="shared" si="8"/>
         <v>3.829802220703693E-2</v>
       </c>
       <c r="L62">
-        <f>ABS(H62-J62)</f>
+        <f t="shared" si="9"/>
         <v>1.4440285955556284E-2</v>
       </c>
     </row>
@@ -13223,23 +12976,23 @@
         <v>0.11625006496560364</v>
       </c>
       <c r="H63">
-        <f>AVERAGE(B63:F63)</f>
+        <f t="shared" si="5"/>
         <v>7.9293874743106244E-2</v>
       </c>
       <c r="I63">
-        <f>MAX(B63:F63)</f>
+        <f t="shared" si="6"/>
         <v>0.11625006496560364</v>
       </c>
       <c r="J63">
-        <f>MIN(B63:F63)</f>
+        <f t="shared" si="7"/>
         <v>6.5771184167855712E-2</v>
       </c>
       <c r="K63">
-        <f>ABS(I63-H63)</f>
+        <f t="shared" si="8"/>
         <v>3.6956190222497395E-2</v>
       </c>
       <c r="L63">
-        <f>ABS(H63-J63)</f>
+        <f t="shared" si="9"/>
         <v>1.3522690575250532E-2</v>
       </c>
     </row>
@@ -13263,23 +13016,23 @@
         <v>0.11220927365710698</v>
       </c>
       <c r="H64">
-        <f>AVERAGE(B64:F64)</f>
+        <f t="shared" si="5"/>
         <v>7.7312420756848355E-2</v>
       </c>
       <c r="I64">
-        <f>MAX(B64:F64)</f>
+        <f t="shared" si="6"/>
         <v>0.11220927365710698</v>
       </c>
       <c r="J64">
-        <f>MIN(B64:F64)</f>
+        <f t="shared" si="7"/>
         <v>6.374845427512478E-2</v>
       </c>
       <c r="K64">
-        <f>ABS(I64-H64)</f>
+        <f t="shared" si="8"/>
         <v>3.4896852900258624E-2</v>
       </c>
       <c r="L64">
-        <f>ABS(H64-J64)</f>
+        <f t="shared" si="9"/>
         <v>1.3563966481723574E-2</v>
       </c>
     </row>
@@ -13303,23 +13056,23 @@
         <v>0.11005032730412845</v>
       </c>
       <c r="H65">
-        <f>AVERAGE(B65:F65)</f>
+        <f t="shared" si="5"/>
         <v>7.7731041798783124E-2</v>
       </c>
       <c r="I65">
-        <f>MAX(B65:F65)</f>
+        <f t="shared" si="6"/>
         <v>0.11005032730412845</v>
       </c>
       <c r="J65">
-        <f>MIN(B65:F65)</f>
+        <f t="shared" si="7"/>
         <v>6.3561673686044123E-2</v>
       </c>
       <c r="K65">
-        <f>ABS(I65-H65)</f>
+        <f t="shared" si="8"/>
         <v>3.2319285505345324E-2</v>
       </c>
       <c r="L65">
-        <f>ABS(H65-J65)</f>
+        <f t="shared" si="9"/>
         <v>1.4169368112739E-2</v>
       </c>
     </row>
@@ -13343,23 +13096,23 @@
         <v>0.1120385076795475</v>
       </c>
       <c r="H66">
-        <f>AVERAGE(B66:F66)</f>
+        <f t="shared" si="5"/>
         <v>7.966297574406922E-2</v>
       </c>
       <c r="I66">
-        <f>MAX(B66:F66)</f>
+        <f t="shared" si="6"/>
         <v>0.1120385076795475</v>
       </c>
       <c r="J66">
-        <f>MIN(B66:F66)</f>
+        <f t="shared" si="7"/>
         <v>6.4030640969432437E-2</v>
       </c>
       <c r="K66">
-        <f>ABS(I66-H66)</f>
+        <f t="shared" si="8"/>
         <v>3.2375531935478277E-2</v>
       </c>
       <c r="L66">
-        <f>ABS(H66-J66)</f>
+        <f t="shared" si="9"/>
         <v>1.5632334774636783E-2</v>
       </c>
     </row>
@@ -13383,23 +13136,23 @@
         <v>0.11295109543613066</v>
       </c>
       <c r="H67">
-        <f>AVERAGE(B67:F67)</f>
+        <f t="shared" si="5"/>
         <v>8.3437414620997657E-2</v>
       </c>
       <c r="I67">
-        <f>MAX(B67:F67)</f>
+        <f t="shared" si="6"/>
         <v>0.11295109543613066</v>
       </c>
       <c r="J67">
-        <f>MIN(B67:F67)</f>
+        <f t="shared" si="7"/>
         <v>7.1592194942437237E-2</v>
       </c>
       <c r="K67">
-        <f>ABS(I67-H67)</f>
+        <f t="shared" si="8"/>
         <v>2.9513680815133003E-2</v>
       </c>
       <c r="L67">
-        <f>ABS(H67-J67)</f>
+        <f t="shared" si="9"/>
         <v>1.184521967856042E-2</v>
       </c>
     </row>
@@ -13423,23 +13176,23 @@
         <v>0.11179484354681317</v>
       </c>
       <c r="H68">
-        <f>AVERAGE(B68:F68)</f>
+        <f t="shared" si="5"/>
         <v>8.3152926012750011E-2</v>
       </c>
       <c r="I68">
-        <f>MAX(B68:F68)</f>
+        <f t="shared" si="6"/>
         <v>0.11179484354681317</v>
       </c>
       <c r="J68">
-        <f>MIN(B68:F68)</f>
+        <f t="shared" si="7"/>
         <v>7.0410884873810017E-2</v>
       </c>
       <c r="K68">
-        <f>ABS(I68-H68)</f>
+        <f t="shared" si="8"/>
         <v>2.8641917534063158E-2</v>
       </c>
       <c r="L68">
-        <f>ABS(H68-J68)</f>
+        <f t="shared" si="9"/>
         <v>1.2742041138939994E-2</v>
       </c>
     </row>
@@ -13454,8 +13207,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5C2E2BE-7ABF-4851-8DBA-2D7EAB1F74AC}">
   <dimension ref="A1:Y120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V31" sqref="V31"/>
+    <sheetView topLeftCell="F4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="S29" sqref="S29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17320,23 +17073,23 @@
         <v>0.64359122963641424</v>
       </c>
       <c r="I93">
-        <f>AVERAGE(C93:G93)</f>
+        <f t="shared" ref="I93:I120" si="25">AVERAGE(C93:G93)</f>
         <v>0.64568106118448676</v>
       </c>
       <c r="J93">
-        <f>MAX(C93:G93)</f>
+        <f t="shared" ref="J93:J120" si="26">MAX(C93:G93)</f>
         <v>0.65564727813074009</v>
       </c>
       <c r="K93">
-        <f>MIN(C93:G93)</f>
+        <f t="shared" ref="K93:K120" si="27">MIN(C93:G93)</f>
         <v>0.64177566299251054</v>
       </c>
       <c r="L93">
-        <f>ABS(J93-I93)</f>
+        <f t="shared" ref="L93:L120" si="28">ABS(J93-I93)</f>
         <v>9.9662169462533257E-3</v>
       </c>
       <c r="M93">
-        <f>ABS(I93-K93)</f>
+        <f t="shared" ref="M93:M120" si="29">ABS(I93-K93)</f>
         <v>3.9053981919762171E-3</v>
       </c>
     </row>
@@ -17345,7 +17098,7 @@
         <v>5000</v>
       </c>
       <c r="B94">
-        <f t="shared" ref="B94:B120" si="25">A94+$A$92+$A$76</f>
+        <f t="shared" ref="B94:B120" si="30">A94+$A$92+$A$76</f>
         <v>125345</v>
       </c>
       <c r="C94" s="1">
@@ -17364,23 +17117,23 @@
         <v>0.16992503113262636</v>
       </c>
       <c r="I94">
-        <f>AVERAGE(C94:G94)</f>
+        <f t="shared" si="25"/>
         <v>0.16566463441515528</v>
       </c>
       <c r="J94">
-        <f>MAX(C94:G94)</f>
+        <f t="shared" si="26"/>
         <v>0.17121379190447522</v>
       </c>
       <c r="K94">
-        <f>MIN(C94:G94)</f>
+        <f t="shared" si="27"/>
         <v>0.15741455225269102</v>
       </c>
       <c r="L94">
-        <f>ABS(J94-I94)</f>
+        <f t="shared" si="28"/>
         <v>5.5491574893199447E-3</v>
       </c>
       <c r="M94">
-        <f>ABS(I94-K94)</f>
+        <f t="shared" si="29"/>
         <v>8.2500821624642562E-3</v>
       </c>
     </row>
@@ -17389,7 +17142,7 @@
         <v>10000</v>
       </c>
       <c r="B95">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>130345</v>
       </c>
       <c r="C95" s="1">
@@ -17408,23 +17161,23 @@
         <v>0.14947191945281835</v>
       </c>
       <c r="I95">
-        <f>AVERAGE(C95:G95)</f>
+        <f t="shared" si="25"/>
         <v>0.12853538873704279</v>
       </c>
       <c r="J95">
-        <f>MAX(C95:G95)</f>
+        <f t="shared" si="26"/>
         <v>0.14947191945281835</v>
       </c>
       <c r="K95">
-        <f>MIN(C95:G95)</f>
+        <f t="shared" si="27"/>
         <v>0.10264617716353634</v>
       </c>
       <c r="L95">
-        <f>ABS(J95-I95)</f>
+        <f t="shared" si="28"/>
         <v>2.0936530715775559E-2</v>
       </c>
       <c r="M95">
-        <f>ABS(I95-K95)</f>
+        <f t="shared" si="29"/>
         <v>2.5889211573506446E-2</v>
       </c>
     </row>
@@ -17433,7 +17186,7 @@
         <v>15000</v>
       </c>
       <c r="B96">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>135345</v>
       </c>
       <c r="C96" s="1">
@@ -17452,23 +17205,23 @@
         <v>0.12669043805260077</v>
       </c>
       <c r="I96">
-        <f>AVERAGE(C96:G96)</f>
+        <f t="shared" si="25"/>
         <v>0.10837140668423832</v>
       </c>
       <c r="J96">
-        <f>MAX(C96:G96)</f>
+        <f t="shared" si="26"/>
         <v>0.12669043805260077</v>
       </c>
       <c r="K96">
-        <f>MIN(C96:G96)</f>
+        <f t="shared" si="27"/>
         <v>7.9713555336000372E-2</v>
       </c>
       <c r="L96">
-        <f>ABS(J96-I96)</f>
+        <f t="shared" si="28"/>
         <v>1.8319031368362451E-2</v>
       </c>
       <c r="M96">
-        <f>ABS(I96-K96)</f>
+        <f t="shared" si="29"/>
         <v>2.865785134823795E-2</v>
       </c>
     </row>
@@ -17477,7 +17230,7 @@
         <v>20000</v>
       </c>
       <c r="B97">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>140345</v>
       </c>
       <c r="C97" s="1">
@@ -17496,23 +17249,23 @@
         <v>0.12143039140483111</v>
       </c>
       <c r="I97">
-        <f>AVERAGE(C97:G97)</f>
+        <f t="shared" si="25"/>
         <v>9.7761753825261227E-2</v>
       </c>
       <c r="J97">
-        <f>MAX(C97:G97)</f>
+        <f t="shared" si="26"/>
         <v>0.12143039140483111</v>
       </c>
       <c r="K97">
-        <f>MIN(C97:G97)</f>
+        <f t="shared" si="27"/>
         <v>6.8417949086619065E-2</v>
       </c>
       <c r="L97">
-        <f>ABS(J97-I97)</f>
+        <f t="shared" si="28"/>
         <v>2.3668637579569884E-2</v>
       </c>
       <c r="M97">
-        <f>ABS(I97-K97)</f>
+        <f t="shared" si="29"/>
         <v>2.9343804738642162E-2</v>
       </c>
     </row>
@@ -17521,7 +17274,7 @@
         <v>25000</v>
       </c>
       <c r="B98">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>145345</v>
       </c>
       <c r="C98" s="1">
@@ -17540,23 +17293,23 @@
         <v>0.12590756195532368</v>
       </c>
       <c r="I98">
-        <f>AVERAGE(C98:G98)</f>
+        <f t="shared" si="25"/>
         <v>9.284929006319273E-2</v>
       </c>
       <c r="J98">
-        <f>MAX(C98:G98)</f>
+        <f t="shared" si="26"/>
         <v>0.12590756195532368</v>
       </c>
       <c r="K98">
-        <f>MIN(C98:G98)</f>
+        <f t="shared" si="27"/>
         <v>6.794474290673061E-2</v>
       </c>
       <c r="L98">
-        <f>ABS(J98-I98)</f>
+        <f t="shared" si="28"/>
         <v>3.3058271892130953E-2</v>
       </c>
       <c r="M98">
-        <f>ABS(I98-K98)</f>
+        <f t="shared" si="29"/>
         <v>2.490454715646212E-2</v>
       </c>
     </row>
@@ -17565,7 +17318,7 @@
         <v>30000</v>
       </c>
       <c r="B99">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>150345</v>
       </c>
       <c r="C99" s="1">
@@ -17584,23 +17337,23 @@
         <v>0.13094038112484133</v>
       </c>
       <c r="I99">
-        <f>AVERAGE(C99:G99)</f>
+        <f t="shared" si="25"/>
         <v>9.0771200004250235E-2</v>
       </c>
       <c r="J99">
-        <f>MAX(C99:G99)</f>
+        <f t="shared" si="26"/>
         <v>0.13094038112484133</v>
       </c>
       <c r="K99">
-        <f>MIN(C99:G99)</f>
+        <f t="shared" si="27"/>
         <v>7.0917822402890768E-2</v>
       </c>
       <c r="L99">
-        <f>ABS(J99-I99)</f>
+        <f t="shared" si="28"/>
         <v>4.0169181120591091E-2</v>
       </c>
       <c r="M99">
-        <f>ABS(I99-K99)</f>
+        <f t="shared" si="29"/>
         <v>1.9853377601359468E-2</v>
       </c>
     </row>
@@ -17609,7 +17362,7 @@
         <v>35000</v>
       </c>
       <c r="B100">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>155345</v>
       </c>
       <c r="C100" s="1">
@@ -17628,23 +17381,23 @@
         <v>0.12314099146818808</v>
       </c>
       <c r="I100">
-        <f>AVERAGE(C100:G100)</f>
+        <f t="shared" si="25"/>
         <v>9.1742951929760647E-2</v>
       </c>
       <c r="J100">
-        <f>MAX(C100:G100)</f>
+        <f t="shared" si="26"/>
         <v>0.12314099146818808</v>
       </c>
       <c r="K100">
-        <f>MIN(C100:G100)</f>
+        <f t="shared" si="27"/>
         <v>7.8556081221673665E-2</v>
       </c>
       <c r="L100">
-        <f>ABS(J100-I100)</f>
+        <f t="shared" si="28"/>
         <v>3.139803953842743E-2</v>
       </c>
       <c r="M100">
-        <f>ABS(I100-K100)</f>
+        <f t="shared" si="29"/>
         <v>1.3186870708086981E-2</v>
       </c>
     </row>
@@ -17653,7 +17406,7 @@
         <v>40000</v>
       </c>
       <c r="B101">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>160345</v>
       </c>
       <c r="C101" s="1">
@@ -17672,23 +17425,23 @@
         <v>0.11616672660385111</v>
       </c>
       <c r="I101">
-        <f>AVERAGE(C101:G101)</f>
+        <f t="shared" si="25"/>
         <v>8.8960335990743516E-2</v>
       </c>
       <c r="J101">
-        <f>MAX(C101:G101)</f>
+        <f t="shared" si="26"/>
         <v>0.11616672660385111</v>
       </c>
       <c r="K101">
-        <f>MIN(C101:G101)</f>
+        <f t="shared" si="27"/>
         <v>7.9971420723080847E-2</v>
       </c>
       <c r="L101">
-        <f>ABS(J101-I101)</f>
+        <f t="shared" si="28"/>
         <v>2.7206390613107589E-2</v>
       </c>
       <c r="M101">
-        <f>ABS(I101-K101)</f>
+        <f t="shared" si="29"/>
         <v>8.9889152676626699E-3</v>
       </c>
     </row>
@@ -17697,7 +17450,7 @@
         <v>45000</v>
       </c>
       <c r="B102">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>165345</v>
       </c>
       <c r="C102" s="1">
@@ -17716,23 +17469,23 @@
         <v>0.11964968111296817</v>
       </c>
       <c r="I102">
-        <f>AVERAGE(C102:G102)</f>
+        <f t="shared" si="25"/>
         <v>8.8804280397221283E-2</v>
       </c>
       <c r="J102">
-        <f>MAX(C102:G102)</f>
+        <f t="shared" si="26"/>
         <v>0.11964968111296817</v>
       </c>
       <c r="K102">
-        <f>MIN(C102:G102)</f>
+        <f t="shared" si="27"/>
         <v>8.0014954545267705E-2</v>
       </c>
       <c r="L102">
-        <f>ABS(J102-I102)</f>
+        <f t="shared" si="28"/>
         <v>3.0845400715746887E-2</v>
       </c>
       <c r="M102">
-        <f>ABS(I102-K102)</f>
+        <f t="shared" si="29"/>
         <v>8.7893258519535777E-3</v>
       </c>
     </row>
@@ -17741,7 +17494,7 @@
         <v>50000</v>
       </c>
       <c r="B103">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>170345</v>
       </c>
       <c r="C103" s="1">
@@ -17760,23 +17513,23 @@
         <v>0.11813228196117424</v>
       </c>
       <c r="I103">
-        <f>AVERAGE(C103:G103)</f>
+        <f t="shared" si="25"/>
         <v>8.4537587038640102E-2</v>
       </c>
       <c r="J103">
-        <f>MAX(C103:G103)</f>
+        <f t="shared" si="26"/>
         <v>0.11813228196117424</v>
       </c>
       <c r="K103">
-        <f>MIN(C103:G103)</f>
+        <f t="shared" si="27"/>
         <v>7.4359327357199523E-2</v>
       </c>
       <c r="L103">
-        <f>ABS(J103-I103)</f>
+        <f t="shared" si="28"/>
         <v>3.3594694922534141E-2</v>
       </c>
       <c r="M103">
-        <f>ABS(I103-K103)</f>
+        <f t="shared" si="29"/>
         <v>1.017825968144058E-2</v>
       </c>
     </row>
@@ -17785,7 +17538,7 @@
         <v>55000</v>
       </c>
       <c r="B104">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>175345</v>
       </c>
       <c r="C104" s="1">
@@ -17804,23 +17557,23 @@
         <v>0.1153553204061179</v>
       </c>
       <c r="I104">
-        <f>AVERAGE(C104:G104)</f>
+        <f t="shared" si="25"/>
         <v>8.5279318499298845E-2</v>
       </c>
       <c r="J104">
-        <f>MAX(C104:G104)</f>
+        <f t="shared" si="26"/>
         <v>0.1153553204061179</v>
       </c>
       <c r="K104">
-        <f>MIN(C104:G104)</f>
+        <f t="shared" si="27"/>
         <v>7.4082667872737526E-2</v>
       </c>
       <c r="L104">
-        <f>ABS(J104-I104)</f>
+        <f t="shared" si="28"/>
         <v>3.0076001906819055E-2</v>
       </c>
       <c r="M104">
-        <f>ABS(I104-K104)</f>
+        <f t="shared" si="29"/>
         <v>1.1196650626561319E-2</v>
       </c>
     </row>
@@ -17829,7 +17582,7 @@
         <v>60000</v>
       </c>
       <c r="B105">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>180345</v>
       </c>
       <c r="C105" s="1">
@@ -17848,23 +17601,23 @@
         <v>0.11904813811538423</v>
       </c>
       <c r="I105">
-        <f>AVERAGE(C105:G105)</f>
+        <f t="shared" si="25"/>
         <v>8.3679085254461813E-2</v>
       </c>
       <c r="J105">
-        <f>MAX(C105:G105)</f>
+        <f t="shared" si="26"/>
         <v>0.11904813811538423</v>
       </c>
       <c r="K105">
-        <f>MIN(C105:G105)</f>
+        <f t="shared" si="27"/>
         <v>7.1604680828084563E-2</v>
       </c>
       <c r="L105">
-        <f>ABS(J105-I105)</f>
+        <f t="shared" si="28"/>
         <v>3.5369052860922415E-2</v>
       </c>
       <c r="M105">
-        <f>ABS(I105-K105)</f>
+        <f t="shared" si="29"/>
         <v>1.207440442637725E-2</v>
       </c>
     </row>
@@ -17873,7 +17626,7 @@
         <v>65000</v>
       </c>
       <c r="B106">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>185345</v>
       </c>
       <c r="C106" s="1">
@@ -17892,23 +17645,23 @@
         <v>0.11779058480724172</v>
       </c>
       <c r="I106">
-        <f>AVERAGE(C106:G106)</f>
+        <f t="shared" si="25"/>
         <v>8.3342137837353919E-2</v>
       </c>
       <c r="J106">
-        <f>MAX(C106:G106)</f>
+        <f t="shared" si="26"/>
         <v>0.11779058480724172</v>
       </c>
       <c r="K106">
-        <f>MIN(C106:G106)</f>
+        <f t="shared" si="27"/>
         <v>7.0431076365544146E-2</v>
       </c>
       <c r="L106">
-        <f>ABS(J106-I106)</f>
+        <f t="shared" si="28"/>
         <v>3.4448446969887803E-2</v>
       </c>
       <c r="M106">
-        <f>ABS(I106-K106)</f>
+        <f t="shared" si="29"/>
         <v>1.2911061471809773E-2</v>
       </c>
     </row>
@@ -17917,7 +17670,7 @@
         <v>70000</v>
       </c>
       <c r="B107">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>190345</v>
       </c>
       <c r="C107" s="1">
@@ -17936,23 +17689,23 @@
         <v>0.12175346783933219</v>
       </c>
       <c r="I107">
-        <f>AVERAGE(C107:G107)</f>
+        <f t="shared" si="25"/>
         <v>8.2609559674169747E-2</v>
       </c>
       <c r="J107">
-        <f>MAX(C107:G107)</f>
+        <f t="shared" si="26"/>
         <v>0.12175346783933219</v>
       </c>
       <c r="K107">
-        <f>MIN(C107:G107)</f>
+        <f t="shared" si="27"/>
         <v>7.0151991068238412E-2</v>
       </c>
       <c r="L107">
-        <f>ABS(J107-I107)</f>
+        <f t="shared" si="28"/>
         <v>3.9143908165162444E-2</v>
       </c>
       <c r="M107">
-        <f>ABS(I107-K107)</f>
+        <f t="shared" si="29"/>
         <v>1.2457568605931335E-2</v>
       </c>
     </row>
@@ -17961,7 +17714,7 @@
         <v>75000</v>
       </c>
       <c r="B108">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>195345</v>
       </c>
       <c r="C108" s="1">
@@ -17980,23 +17733,23 @@
         <v>0.11486732760285613</v>
       </c>
       <c r="I108">
-        <f>AVERAGE(C108:G108)</f>
+        <f t="shared" si="25"/>
         <v>8.1042251220067793E-2</v>
       </c>
       <c r="J108">
-        <f>MAX(C108:G108)</f>
+        <f t="shared" si="26"/>
         <v>0.11486732760285613</v>
       </c>
       <c r="K108">
-        <f>MIN(C108:G108)</f>
+        <f t="shared" si="27"/>
         <v>6.7781123651443023E-2</v>
       </c>
       <c r="L108">
-        <f>ABS(J108-I108)</f>
+        <f t="shared" si="28"/>
         <v>3.3825076382788338E-2</v>
       </c>
       <c r="M108">
-        <f>ABS(I108-K108)</f>
+        <f t="shared" si="29"/>
         <v>1.326112756862477E-2</v>
       </c>
     </row>
@@ -18005,7 +17758,7 @@
         <v>80000</v>
       </c>
       <c r="B109">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>200345</v>
       </c>
       <c r="C109" s="1">
@@ -18024,23 +17777,23 @@
         <v>0.12027878537929701</v>
       </c>
       <c r="I109">
-        <f>AVERAGE(C109:G109)</f>
+        <f t="shared" si="25"/>
         <v>8.1644820982847005E-2</v>
       </c>
       <c r="J109">
-        <f>MAX(C109:G109)</f>
+        <f t="shared" si="26"/>
         <v>0.12027878537929701</v>
       </c>
       <c r="K109">
-        <f>MIN(C109:G109)</f>
+        <f t="shared" si="27"/>
         <v>6.6308122882500528E-2</v>
       </c>
       <c r="L109">
-        <f>ABS(J109-I109)</f>
+        <f t="shared" si="28"/>
         <v>3.8633964396450005E-2</v>
       </c>
       <c r="M109">
-        <f>ABS(I109-K109)</f>
+        <f t="shared" si="29"/>
         <v>1.5336698100346477E-2</v>
       </c>
     </row>
@@ -18049,7 +17802,7 @@
         <v>85000</v>
       </c>
       <c r="B110">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>205345</v>
       </c>
       <c r="C110" s="1">
@@ -18068,23 +17821,23 @@
         <v>0.11858769496918496</v>
       </c>
       <c r="I110">
-        <f>AVERAGE(C110:G110)</f>
+        <f t="shared" si="25"/>
         <v>8.1467829886864462E-2</v>
       </c>
       <c r="J110">
-        <f>MAX(C110:G110)</f>
+        <f t="shared" si="26"/>
         <v>0.11858769496918496</v>
       </c>
       <c r="K110">
-        <f>MIN(C110:G110)</f>
+        <f t="shared" si="27"/>
         <v>6.6511157585873573E-2</v>
       </c>
       <c r="L110">
-        <f>ABS(J110-I110)</f>
+        <f t="shared" si="28"/>
         <v>3.71198650823205E-2</v>
       </c>
       <c r="M110">
-        <f>ABS(I110-K110)</f>
+        <f t="shared" si="29"/>
         <v>1.4956672300990889E-2</v>
       </c>
     </row>
@@ -18093,7 +17846,7 @@
         <v>90000</v>
       </c>
       <c r="B111">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>210345</v>
       </c>
       <c r="C111" s="1">
@@ -18112,23 +17865,23 @@
         <v>0.11586210826727643</v>
       </c>
       <c r="I111">
-        <f>AVERAGE(C111:G111)</f>
+        <f t="shared" si="25"/>
         <v>7.9487300106056077E-2</v>
       </c>
       <c r="J111">
-        <f>MAX(C111:G111)</f>
+        <f t="shared" si="26"/>
         <v>0.11586210826727643</v>
       </c>
       <c r="K111">
-        <f>MIN(C111:G111)</f>
+        <f t="shared" si="27"/>
         <v>6.7591309555555715E-2</v>
       </c>
       <c r="L111">
-        <f>ABS(J111-I111)</f>
+        <f t="shared" si="28"/>
         <v>3.6374808161220351E-2</v>
       </c>
       <c r="M111">
-        <f>ABS(I111-K111)</f>
+        <f t="shared" si="29"/>
         <v>1.1895990550500363E-2</v>
       </c>
     </row>
@@ -18137,7 +17890,7 @@
         <v>95000</v>
       </c>
       <c r="B112">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>215345</v>
       </c>
       <c r="C112" s="1">
@@ -18156,23 +17909,23 @@
         <v>0.11770675149515496</v>
       </c>
       <c r="I112">
-        <f>AVERAGE(C112:G112)</f>
+        <f t="shared" si="25"/>
         <v>7.9577212207535691E-2</v>
       </c>
       <c r="J112">
-        <f>MAX(C112:G112)</f>
+        <f t="shared" si="26"/>
         <v>0.11770675149515496</v>
       </c>
       <c r="K112">
-        <f>MIN(C112:G112)</f>
+        <f t="shared" si="27"/>
         <v>6.6131741889763632E-2</v>
       </c>
       <c r="L112">
-        <f>ABS(J112-I112)</f>
+        <f t="shared" si="28"/>
         <v>3.8129539287619266E-2</v>
       </c>
       <c r="M112">
-        <f>ABS(I112-K112)</f>
+        <f t="shared" si="29"/>
         <v>1.344547031777206E-2</v>
       </c>
     </row>
@@ -18181,7 +17934,7 @@
         <v>100000</v>
       </c>
       <c r="B113">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>220345</v>
       </c>
       <c r="C113" s="1">
@@ -18200,23 +17953,23 @@
         <v>0.11543658368835599</v>
       </c>
       <c r="I113">
-        <f>AVERAGE(C113:G113)</f>
+        <f t="shared" si="25"/>
         <v>7.8332492517794977E-2</v>
       </c>
       <c r="J113">
-        <f>MAX(C113:G113)</f>
+        <f t="shared" si="26"/>
         <v>0.11543658368835599</v>
       </c>
       <c r="K113">
-        <f>MIN(C113:G113)</f>
+        <f t="shared" si="27"/>
         <v>6.4811161956278465E-2</v>
       </c>
       <c r="L113">
-        <f>ABS(J113-I113)</f>
+        <f t="shared" si="28"/>
         <v>3.7104091170561015E-2</v>
       </c>
       <c r="M113">
-        <f>ABS(I113-K113)</f>
+        <f t="shared" si="29"/>
         <v>1.3521330561516512E-2</v>
       </c>
     </row>
@@ -18225,7 +17978,7 @@
         <v>105000</v>
       </c>
       <c r="B114">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>225345</v>
       </c>
       <c r="C114" s="1">
@@ -18244,23 +17997,23 @@
         <v>0.11814605262891359</v>
       </c>
       <c r="I114">
-        <f>AVERAGE(C114:G114)</f>
+        <f t="shared" si="25"/>
         <v>7.9848030421876659E-2</v>
       </c>
       <c r="J114">
-        <f>MAX(C114:G114)</f>
+        <f t="shared" si="26"/>
         <v>0.11814605262891359</v>
       </c>
       <c r="K114">
-        <f>MIN(C114:G114)</f>
+        <f t="shared" si="27"/>
         <v>6.5407744466320375E-2</v>
       </c>
       <c r="L114">
-        <f>ABS(J114-I114)</f>
+        <f t="shared" si="28"/>
         <v>3.829802220703693E-2</v>
       </c>
       <c r="M114">
-        <f>ABS(I114-K114)</f>
+        <f t="shared" si="29"/>
         <v>1.4440285955556284E-2</v>
       </c>
     </row>
@@ -18269,7 +18022,7 @@
         <v>110000</v>
       </c>
       <c r="B115">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>230345</v>
       </c>
       <c r="C115" s="1">
@@ -18288,23 +18041,23 @@
         <v>0.11625006496560364</v>
       </c>
       <c r="I115">
-        <f>AVERAGE(C115:G115)</f>
+        <f t="shared" si="25"/>
         <v>7.9293874743106244E-2</v>
       </c>
       <c r="J115">
-        <f>MAX(C115:G115)</f>
+        <f t="shared" si="26"/>
         <v>0.11625006496560364</v>
       </c>
       <c r="K115">
-        <f>MIN(C115:G115)</f>
+        <f t="shared" si="27"/>
         <v>6.5771184167855712E-2</v>
       </c>
       <c r="L115">
-        <f>ABS(J115-I115)</f>
+        <f t="shared" si="28"/>
         <v>3.6956190222497395E-2</v>
       </c>
       <c r="M115">
-        <f>ABS(I115-K115)</f>
+        <f t="shared" si="29"/>
         <v>1.3522690575250532E-2</v>
       </c>
     </row>
@@ -18313,7 +18066,7 @@
         <v>115000</v>
       </c>
       <c r="B116">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>235345</v>
       </c>
       <c r="C116" s="1">
@@ -18332,23 +18085,23 @@
         <v>0.11220927365710698</v>
       </c>
       <c r="I116">
-        <f>AVERAGE(C116:G116)</f>
+        <f t="shared" si="25"/>
         <v>7.7312420756848355E-2</v>
       </c>
       <c r="J116">
-        <f>MAX(C116:G116)</f>
+        <f t="shared" si="26"/>
         <v>0.11220927365710698</v>
       </c>
       <c r="K116">
-        <f>MIN(C116:G116)</f>
+        <f t="shared" si="27"/>
         <v>6.374845427512478E-2</v>
       </c>
       <c r="L116">
-        <f>ABS(J116-I116)</f>
+        <f t="shared" si="28"/>
         <v>3.4896852900258624E-2</v>
       </c>
       <c r="M116">
-        <f>ABS(I116-K116)</f>
+        <f t="shared" si="29"/>
         <v>1.3563966481723574E-2</v>
       </c>
     </row>
@@ -18357,7 +18110,7 @@
         <v>120000</v>
       </c>
       <c r="B117">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>240345</v>
       </c>
       <c r="C117" s="1">
@@ -18376,23 +18129,23 @@
         <v>0.11005032730412845</v>
       </c>
       <c r="I117">
-        <f>AVERAGE(C117:G117)</f>
+        <f t="shared" si="25"/>
         <v>7.7731041798783124E-2</v>
       </c>
       <c r="J117">
-        <f>MAX(C117:G117)</f>
+        <f t="shared" si="26"/>
         <v>0.11005032730412845</v>
       </c>
       <c r="K117">
-        <f>MIN(C117:G117)</f>
+        <f t="shared" si="27"/>
         <v>6.3561673686044123E-2</v>
       </c>
       <c r="L117">
-        <f>ABS(J117-I117)</f>
+        <f t="shared" si="28"/>
         <v>3.2319285505345324E-2</v>
       </c>
       <c r="M117">
-        <f>ABS(I117-K117)</f>
+        <f t="shared" si="29"/>
         <v>1.4169368112739E-2</v>
       </c>
     </row>
@@ -18401,7 +18154,7 @@
         <v>125000</v>
       </c>
       <c r="B118">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>245345</v>
       </c>
       <c r="C118" s="1">
@@ -18420,23 +18173,23 @@
         <v>0.1120385076795475</v>
       </c>
       <c r="I118">
-        <f>AVERAGE(C118:G118)</f>
+        <f t="shared" si="25"/>
         <v>7.966297574406922E-2</v>
       </c>
       <c r="J118">
-        <f>MAX(C118:G118)</f>
+        <f t="shared" si="26"/>
         <v>0.1120385076795475</v>
       </c>
       <c r="K118">
-        <f>MIN(C118:G118)</f>
+        <f t="shared" si="27"/>
         <v>6.4030640969432437E-2</v>
       </c>
       <c r="L118">
-        <f>ABS(J118-I118)</f>
+        <f t="shared" si="28"/>
         <v>3.2375531935478277E-2</v>
       </c>
       <c r="M118">
-        <f>ABS(I118-K118)</f>
+        <f t="shared" si="29"/>
         <v>1.5632334774636783E-2</v>
       </c>
     </row>
@@ -18445,7 +18198,7 @@
         <v>130000</v>
       </c>
       <c r="B119">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>250345</v>
       </c>
       <c r="C119" s="1">
@@ -18464,23 +18217,23 @@
         <v>0.11295109543613066</v>
       </c>
       <c r="I119">
-        <f>AVERAGE(C119:G119)</f>
+        <f t="shared" si="25"/>
         <v>8.3437414620997657E-2</v>
       </c>
       <c r="J119">
-        <f>MAX(C119:G119)</f>
+        <f t="shared" si="26"/>
         <v>0.11295109543613066</v>
       </c>
       <c r="K119">
-        <f>MIN(C119:G119)</f>
+        <f t="shared" si="27"/>
         <v>7.1592194942437237E-2</v>
       </c>
       <c r="L119">
-        <f>ABS(J119-I119)</f>
+        <f t="shared" si="28"/>
         <v>2.9513680815133003E-2</v>
       </c>
       <c r="M119">
-        <f>ABS(I119-K119)</f>
+        <f t="shared" si="29"/>
         <v>1.184521967856042E-2</v>
       </c>
     </row>
@@ -18489,7 +18242,7 @@
         <v>131189</v>
       </c>
       <c r="B120">
-        <f t="shared" si="25"/>
+        <f t="shared" si="30"/>
         <v>251534</v>
       </c>
       <c r="C120" s="1">
@@ -18508,23 +18261,23 @@
         <v>0.11179484354681317</v>
       </c>
       <c r="I120">
-        <f>AVERAGE(C120:G120)</f>
+        <f t="shared" si="25"/>
         <v>8.3152926012750011E-2</v>
       </c>
       <c r="J120">
-        <f>MAX(C120:G120)</f>
+        <f t="shared" si="26"/>
         <v>0.11179484354681317</v>
       </c>
       <c r="K120">
-        <f>MIN(C120:G120)</f>
+        <f t="shared" si="27"/>
         <v>7.0410884873810017E-2</v>
       </c>
       <c r="L120">
-        <f>ABS(J120-I120)</f>
+        <f t="shared" si="28"/>
         <v>2.8641917534063158E-2</v>
       </c>
       <c r="M120">
-        <f>ABS(I120-K120)</f>
+        <f t="shared" si="29"/>
         <v>1.2742041138939994E-2</v>
       </c>
     </row>

</xml_diff>